<commit_message>
Update bug fixes for home page icons, filter menu and forms
</commit_message>
<xml_diff>
--- a/testing/testing.xlsx
+++ b/testing/testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c2d4706cdffd893/3. EDUCATION/FULLSTACK SOFTWARE DEVELOPMENT DIPLOMA/MS-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{67B22251-1CDE-4A42-BE5A-D1762AAEA8FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A72817DB-7ACE-477A-9E45-63202609E698}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{67B22251-1CDE-4A42-BE5A-D1762AAEA8FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E35686B-4625-41B6-9C9B-C97729ADB435}"/>
   <bookViews>
-    <workbookView xWindow="-270" yWindow="0" windowWidth="29070" windowHeight="15600" activeTab="2" xr2:uid="{5A23EB50-F6EE-45F3-A5F7-94914E52C60F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5A23EB50-F6EE-45F3-A5F7-94914E52C60F}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="135">
   <si>
     <t>Test Criteria &amp; Features</t>
   </si>
@@ -420,6 +420,42 @@
   </si>
   <si>
     <t>1. A black background with white fields and a transparent button. 2. Name, email, mobile number, product type, quantity and text area input fields. 3.Mandatory fields that display an error message if content is missing or incorrect on submission. 4. The border is  yellow and of a 1-2px weight when hovered over. 5.A submission button with a Send it! value. 6. A submission button that is yellow on hover. 7. A modal message for successfull or unsuccessful submission</t>
+  </si>
+  <si>
+    <t>Order Form to send emails via EmailJS</t>
+  </si>
+  <si>
+    <t>412 Error found in the console: "Preconditioned Fail"</t>
+  </si>
+  <si>
+    <t>Homepage Icons to be clickable to display company information</t>
+  </si>
+  <si>
+    <t>First click attempt not functioning and general design not condusive to good UX</t>
+  </si>
+  <si>
+    <t>Removed JS onClick functionality and replaced with CSS on hover pseudo class</t>
+  </si>
+  <si>
+    <t>Filter buttons to highlight yellow when active</t>
+  </si>
+  <si>
+    <t>All products button staying highlighed when others were in use</t>
+  </si>
+  <si>
+    <t>1. Remove currentBtnClickListner function from being declared as a variable.</t>
+  </si>
+  <si>
+    <t>Forms to handle invalid or empty inputs</t>
+  </si>
+  <si>
+    <t>Forms accepting empty white space in fields</t>
+  </si>
+  <si>
+    <t>1.Submission failed despite required attribute present in inputs fields &amp; JS validating against empty or one escape entered. I added an extensive JS function to validate all fields which triggers a modal on submission if an error is present, .trim method used to remove empty spaces.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Opened emailJS platform and advised by alert to reconnect my email, so deleted it and re-added it. Issue appears to be resolved. Researched &amp; contacted tutor support to find out the cause of the error but they were not familiar with it or how to prevent it in future. Suspect it is caused by the EmailJS platform and outside my code's control. A modal is present to alert the user that their submission failed, I tested it by altering the API Key and it appeared/was called successfully. </t>
   </si>
 </sst>
 </file>
@@ -644,29 +680,29 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -722,15 +758,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>388621</xdr:colOff>
+      <xdr:colOff>363673</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2580718</xdr:rowOff>
+      <xdr:rowOff>2360736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1824173</xdr:colOff>
+      <xdr:colOff>1826440</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>5063490</xdr:rowOff>
+      <xdr:rowOff>4843508</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -759,8 +795,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4634050" y="7139111"/>
-          <a:ext cx="2047873" cy="2482772"/>
+          <a:off x="4609102" y="6823879"/>
+          <a:ext cx="2075088" cy="2482772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1088,14 +1124,14 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1110,11 +1146,11 @@
         <v>2</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="6" t="s">
         <v>86</v>
       </c>
@@ -1139,11 +1175,11 @@
         <v>57</v>
       </c>
       <c r="C5" s="16"/>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="31" t="s">
         <v>58</v>
       </c>
       <c r="E5" s="24"/>
-      <c r="F5" s="26"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="17" t="s">
         <v>59</v>
       </c>
@@ -1167,11 +1203,11 @@
         <v>60</v>
       </c>
       <c r="C7" s="16"/>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="31" t="s">
         <v>61</v>
       </c>
       <c r="E7" s="24"/>
-      <c r="F7" s="26"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="17" t="s">
         <v>3</v>
       </c>
@@ -1195,11 +1231,11 @@
         <v>65</v>
       </c>
       <c r="C9" s="16"/>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="31" t="s">
         <v>66</v>
       </c>
       <c r="E9" s="24"/>
-      <c r="F9" s="26"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="17" t="s">
         <v>3</v>
       </c>
@@ -1223,11 +1259,11 @@
         <v>69</v>
       </c>
       <c r="C11" s="16"/>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="31" t="s">
         <v>70</v>
       </c>
       <c r="E11" s="24"/>
-      <c r="F11" s="26"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="17" t="s">
         <v>3</v>
       </c>
@@ -1318,22 +1354,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1360,14 +1396,14 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1382,11 +1418,11 @@
         <v>4</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="6" t="s">
         <v>86</v>
       </c>
@@ -1480,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7199C696-BAE5-4023-8427-5238B776A8B5}">
   <dimension ref="B1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:F12"/>
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,14 +1533,14 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1519,11 +1555,11 @@
         <v>5</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1576,11 +1612,11 @@
         <v>101</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="31" t="s">
         <v>102</v>
       </c>
       <c r="E7" s="24"/>
-      <c r="F7" s="26"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="12" t="s">
         <v>3</v>
       </c>
@@ -1671,11 +1707,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="B2:G2"/>
@@ -1683,6 +1714,11 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1691,10 +1727,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FACEED-12E5-4B7A-B200-FE4D145D4ADD}">
-  <dimension ref="B1:H16"/>
+  <dimension ref="B1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,15 +1744,15 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
@@ -1726,11 +1762,11 @@
         <v>9</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="20" t="s">
         <v>11</v>
       </c>
@@ -1752,7 +1788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>17</v>
       </c>
@@ -1837,7 +1873,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="384" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
         <v>36</v>
       </c>
@@ -1869,7 +1905,7 @@
       <c r="G11" s="39"/>
       <c r="H11" s="40"/>
     </row>
-    <row r="12" spans="2:8" ht="106.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>45</v>
       </c>
@@ -1877,11 +1913,11 @@
         <v>44</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="31" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="24"/>
-      <c r="G12" s="26"/>
+      <c r="G12" s="32"/>
       <c r="H12" s="22" t="s">
         <v>47</v>
       </c>
@@ -1894,11 +1930,11 @@
         <v>49</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="31" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="24"/>
-      <c r="G13" s="26"/>
+      <c r="G13" s="32"/>
       <c r="H13" s="22" t="s">
         <v>51</v>
       </c>
@@ -1926,11 +1962,11 @@
         <v>114</v>
       </c>
       <c r="D15" s="8"/>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="31" t="s">
         <v>115</v>
       </c>
       <c r="F15" s="24"/>
-      <c r="G15" s="26"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="22" t="s">
         <v>120</v>
       </c>
@@ -1950,8 +1986,72 @@
       <c r="G16" s="36"/>
       <c r="H16" s="37"/>
     </row>
+    <row r="17" spans="2:8" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+    </row>
+    <row r="18" spans="2:8" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
+    </row>
+    <row r="19" spans="2:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
+    </row>
+    <row r="20" spans="2:8" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="19">
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
     <mergeCell ref="E16:H16"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E11:H11"/>

</xml_diff>